<commit_message>
two images were left out and now added.
</commit_message>
<xml_diff>
--- a/datasets/satelliteData/satHsvFinal4.xlsx
+++ b/datasets/satelliteData/satHsvFinal4.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
   <si>
     <t xml:space="preserve">sat_label</t>
   </si>
@@ -174,217 +174,229 @@
     <t xml:space="preserve">Lawrenceville School’s Big Red Farm</t>
   </si>
   <si>
+    <t xml:space="preserve">gray39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">farmStony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/farmStony.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stony Ford Field Station Farm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gardenMtLake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/gardenMtLake.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mt. Lake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">garden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">darkslategray</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gardenPrinceton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/gardenPrinceton.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Princeton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray31</t>
+  </si>
+  <si>
     <t xml:space="preserve">gray20</t>
   </si>
   <si>
-    <t xml:space="preserve">gray12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">farmStony</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/farmStony.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stony Ford Field Station Farm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gardenMtLake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/gardenMtLake.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mt. Lake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">garden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">darkslategray</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gardenPrinceton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/gardenPrinceton.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Princeton</t>
+    <t xml:space="preserve">lemonchiffon4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">golfHopewell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/golfHopewell.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hopewell Golf course</t>
+  </si>
+  <si>
+    <t xml:space="preserve">golf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">golfPrinceton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/golfPrinceton.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Princeton golf course</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ivory4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preserveMtLakes1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/preserveMtLakes1000.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billie Johnson Mountain Lakes Nature Preserve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preserve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">darkseagreen4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preserveMtRose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/preserveMtRose.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mt Rose Preserve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">darkolivegreen4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preserveStonyOctagon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/preserveStonyOctagon.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stony Ford Research Station; Octogon; Preserve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schHopeElem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/schHopeElem.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hopewell Elemenary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">school</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schHopeHS_TimberMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/schHopeHS_TimberMS.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hopewell Central HS + Timberlane MS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schTollGram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/schTollGram.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toll Gate Grammer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">univArtMuseum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/univArtMuseum.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Art Museum; Princton Univ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">univ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lightyellow4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">univForestSwTrack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/univForestSwTrack.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forest; SW Track and Jadwin Gym; Princeton Univ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">univGuyotHall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/univGuyotHall.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guyot Hall; Princeton Univ</t>
   </si>
   <si>
     <t xml:space="preserve">gray32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cornsilk4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">golfHopewell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/golfHopewell.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hopewell Golf course</t>
-  </si>
-  <si>
-    <t xml:space="preserve">golf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lemonchiffon4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">golfPrinceton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/golfPrinceton.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Princeton golf course</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ivory4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preserveMtLakes1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/preserveMtLakes1000.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billie Johnson Mountain Lakes Nature Preserve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preserve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">darkseagreen4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preserveMtRose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/preserveMtRose.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mt Rose Preserve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">darkolivegreen4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schHopeElem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/schHopeElem.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hopewell Elemenary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">school</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schHopeHS_TimberMS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/schHopeHS_TimberMS.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hopewell Central HS + Timberlane MS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schTollGram</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/schTollGram.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Toll Gate Grammer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">univArtMuseum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/univArtMuseum.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Art Museum; Princton Univ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">univ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lightyellow4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">univForestSwTrack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/univForestSwTrack.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forest; SW Track and Jadwin Gym; Princeton Univ</t>
   </si>
   <si>
     <t xml:space="preserve">univSolarFarm</t>
@@ -960,10 +972,10 @@
         <v>0.141224106808261</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.385538958490669</v>
+        <v>0.385536488149167</v>
       </c>
       <c r="R2" t="n">
-        <v>0.269805970565836</v>
+        <v>0.269805078863159</v>
       </c>
       <c r="S2" t="n">
         <v>0.184052463727089</v>
@@ -972,10 +984,10 @@
         <v>0.758265641273835</v>
       </c>
       <c r="U2" t="n">
-        <v>0.411357537332488</v>
+        <v>0.411359962305478</v>
       </c>
       <c r="V2" t="n">
-        <v>0.457602108829352</v>
+        <v>0.457600622271955</v>
       </c>
       <c r="W2" t="n">
         <v>0.228493221963286</v>
@@ -984,10 +996,10 @@
         <v>0.0971355413606805</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.218272044407381</v>
+        <v>0.218273582891802</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.423721372267061</v>
+        <v>0.423726603932</v>
       </c>
       <c r="AA2" t="n">
         <v>0.502912059019697</v>
@@ -996,10 +1008,10 @@
         <v>0.472962536157234</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.470394337714863</v>
+        <v>0.470407206544719</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.36704292673959</v>
+        <v>0.367030057909734</v>
       </c>
       <c r="AE2" t="n">
         <v>0.137788399669087</v>
@@ -1070,52 +1082,52 @@
         <v>0.136411781841319</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.348304066709259</v>
+        <v>0.348399319418516</v>
       </c>
       <c r="R3" t="n">
-        <v>0.277829925204662</v>
+        <v>0.27784732799299</v>
       </c>
       <c r="S3" t="n">
-        <v>0.192623123868157</v>
+        <v>0.19267140628594</v>
       </c>
       <c r="T3" t="n">
-        <v>0.768186494757718</v>
+        <v>0.768234550270837</v>
       </c>
       <c r="U3" t="n">
-        <v>0.403185526498328</v>
+        <v>0.402966035288512</v>
       </c>
       <c r="V3" t="n">
-        <v>0.462868137645156</v>
+        <v>0.463101953310469</v>
       </c>
       <c r="W3" t="n">
-        <v>0.24791766775556</v>
+        <v>0.248102325074812</v>
       </c>
       <c r="X3" t="n">
-        <v>0.122473468447668</v>
+        <v>0.122429261787393</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.197970550151593</v>
+        <v>0.197951740525308</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.378635750892817</v>
+        <v>0.378367451507324</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.456042495820147</v>
+        <v>0.456042444462877</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.429203985196606</v>
+        <v>0.429280782048271</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.438714955418697</v>
+        <v>0.438251677543892</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.354177773692435</v>
+        <v>0.354431473481018</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.166996966632963</v>
+        <v>0.167219413549039</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.0401103042559059</v>
+        <v>0.0400974354260502</v>
       </c>
       <c r="AG3" t="s">
         <v>47</v>
@@ -1180,75 +1192,75 @@
         <v>0.128242280226708</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.244185052469365</v>
+        <v>0.378236670198313</v>
       </c>
       <c r="R4" t="n">
-        <v>0.334440189526422</v>
+        <v>0.270752677245677</v>
       </c>
       <c r="S4" t="n">
-        <v>0.447154739516437</v>
+        <v>0.218552832601801</v>
       </c>
       <c r="T4" t="n">
-        <v>0.739945514355679</v>
+        <v>0.743408040722596</v>
       </c>
       <c r="U4" t="n">
-        <v>0.402459359815953</v>
+        <v>0.426989070875266</v>
       </c>
       <c r="V4" t="n">
-        <v>0.402609408507201</v>
+        <v>0.46601456885033</v>
       </c>
       <c r="W4" t="n">
-        <v>0.465063438823115</v>
+        <v>0.26042002428372</v>
       </c>
       <c r="X4" t="n">
-        <v>0.106360045366551</v>
+        <v>0.111349519423323</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.452819285787554</v>
+        <v>0.219968537308021</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.274006890509139</v>
+        <v>0.429028028111778</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.146034646242736</v>
+        <v>0.438953171422318</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.420038896638801</v>
+        <v>0.414093728463129</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.471576431657321</v>
+        <v>0.412684989429175</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.372947881239084</v>
+        <v>0.382549866715691</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.134234764224653</v>
+        <v>0.183424947145877</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.0212409228789411</v>
+        <v>0.0213401967092564</v>
       </c>
       <c r="AG4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH4" t="s">
         <v>41</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
         <v>53</v>
       </c>
-      <c r="AI4" t="s">
-        <v>54</v>
-      </c>
       <c r="AJ4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
         <v>55</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>56</v>
-      </c>
-      <c r="C5" t="s">
-        <v>57</v>
       </c>
       <c r="D5" t="s">
         <v>39</v>
@@ -1290,78 +1302,78 @@
         <v>0.136279722924118</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.379734376620002</v>
+        <v>0.37961453231836</v>
       </c>
       <c r="R5" t="n">
-        <v>0.280779349365682</v>
+        <v>0.280721337264827</v>
       </c>
       <c r="S5" t="n">
-        <v>0.187858675071881</v>
+        <v>0.187757607754354</v>
       </c>
       <c r="T5" t="n">
-        <v>0.775050840819737</v>
+        <v>0.775034535247682</v>
       </c>
       <c r="U5" t="n">
-        <v>0.375429326599417</v>
+        <v>0.375586942757632</v>
       </c>
       <c r="V5" t="n">
-        <v>0.466365749127651</v>
+        <v>0.466275393892707</v>
       </c>
       <c r="W5" t="n">
-        <v>0.25028820553429</v>
+        <v>0.250026745501884</v>
       </c>
       <c r="X5" t="n">
-        <v>0.112375368584235</v>
+        <v>0.112384389496513</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.189535249712218</v>
+        <v>0.189560197910951</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.350888410212513</v>
+        <v>0.351171178127506</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.465868934884591</v>
+        <v>0.465924329403919</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.446852499558382</v>
+        <v>0.446826682492629</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.428210313447927</v>
+        <v>0.428826178876735</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.403689677360051</v>
+        <v>0.403349572571008</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.132389006342495</v>
+        <v>0.1321095688942</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.0357110028495266</v>
+        <v>0.0357146796580568</v>
       </c>
       <c r="AG5" t="s">
         <v>47</v>
       </c>
       <c r="AH5" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="AI5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AJ5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
         <v>60</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>61</v>
-      </c>
-      <c r="C6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" t="s">
-        <v>63</v>
       </c>
       <c r="E6" t="n">
         <v>40.365934</v>
@@ -1400,78 +1412,78 @@
         <v>0.135161968799217</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.362378031017664</v>
+        <v>0.362383872521582</v>
       </c>
       <c r="R6" t="n">
-        <v>0.500370779355212</v>
+        <v>0.500389745714076</v>
       </c>
       <c r="S6" t="n">
-        <v>0.240178135255276</v>
+        <v>0.240184213816329</v>
       </c>
       <c r="T6" t="n">
         <v>0.687650725398028</v>
       </c>
       <c r="U6" t="n">
-        <v>0.319258964610822</v>
+        <v>0.319270292188147</v>
       </c>
       <c r="V6" t="n">
-        <v>0.387294412924983</v>
+        <v>0.38729163908905</v>
       </c>
       <c r="W6" t="n">
-        <v>0.181108538341975</v>
+        <v>0.181111585767093</v>
       </c>
       <c r="X6" t="n">
         <v>0.0958285240958132</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.353423647100445</v>
+        <v>0.353415612746418</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.220718759573085</v>
+        <v>0.220703335260754</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.51728731497723</v>
+        <v>0.517280857042752</v>
       </c>
       <c r="AB6" t="n">
         <v>0.546007421579363</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.476284584980237</v>
+        <v>0.476326868278334</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.261700523945216</v>
+        <v>0.261647210221528</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.157898703924993</v>
+        <v>0.157909734350584</v>
       </c>
       <c r="AF6" t="n">
         <v>0.104116187149554</v>
       </c>
       <c r="AG6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI6" t="s">
         <v>64</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AJ6" t="s">
         <v>65</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
         <v>68</v>
       </c>
-      <c r="B7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" t="s">
-        <v>70</v>
-      </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E7" t="n">
         <v>40.347059</v>
@@ -1510,78 +1522,78 @@
         <v>0.141336961844477</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.368804034382226</v>
+        <v>0.378449003640395</v>
       </c>
       <c r="R7" t="n">
-        <v>0.540333760598456</v>
+        <v>0.542971395077246</v>
       </c>
       <c r="S7" t="n">
-        <v>0.221063536378446</v>
+        <v>0.225363593168575</v>
       </c>
       <c r="T7" t="n">
-        <v>0.698919899052576</v>
+        <v>0.699342372843117</v>
       </c>
       <c r="U7" t="n">
-        <v>0.271197822819021</v>
+        <v>0.271980705841052</v>
       </c>
       <c r="V7" t="n">
-        <v>0.363194527338301</v>
+        <v>0.374500758063418</v>
       </c>
       <c r="W7" t="n">
-        <v>0.148692061374659</v>
+        <v>0.153632979216308</v>
       </c>
       <c r="X7" t="n">
-        <v>0.0912785914911102</v>
+        <v>0.0925204579492771</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.378736424153979</v>
+        <v>0.370722435119189</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.249394561470606</v>
+        <v>0.244852292294164</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.542303778243217</v>
+        <v>0.538342980372586</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.546325179070443</v>
+        <v>0.543221886331469</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.377781046052027</v>
+        <v>0.388272819192941</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.253120691240004</v>
+        <v>0.228460336427981</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.194288077948341</v>
+        <v>0.206335141097527</v>
       </c>
       <c r="AF7" t="n">
-        <v>0.174810184759629</v>
+        <v>0.176931703281552</v>
       </c>
       <c r="AG7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI7" t="s">
         <v>71</v>
       </c>
-      <c r="AH7" t="s">
-        <v>72</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>73</v>
-      </c>
       <c r="AJ7" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" t="s">
         <v>75</v>
-      </c>
-      <c r="B8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" t="s">
-        <v>78</v>
       </c>
       <c r="E8" t="n">
         <v>40.364166</v>
@@ -1620,49 +1632,49 @@
         <v>0.137237314427854</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.301441173100104</v>
+        <v>0.301448007786584</v>
       </c>
       <c r="R8" t="n">
-        <v>0.404116518309816</v>
+        <v>0.404124568183147</v>
       </c>
       <c r="S8" t="n">
-        <v>0.169680265371939</v>
+        <v>0.169684550278726</v>
       </c>
       <c r="T8" t="n">
         <v>0.660106479673258</v>
       </c>
       <c r="U8" t="n">
-        <v>0.362319167846906</v>
+        <v>0.36232169399861</v>
       </c>
       <c r="V8" t="n">
-        <v>0.427690934357832</v>
+        <v>0.427698684951855</v>
       </c>
       <c r="W8" t="n">
-        <v>0.217343585220565</v>
+        <v>0.217352690291093</v>
       </c>
       <c r="X8" t="n">
         <v>0.0930083757348977</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.375706546116317</v>
+        <v>0.375694172149662</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.210056248267792</v>
+        <v>0.210050829920029</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.528070881660251</v>
+        <v>0.528062208558599</v>
       </c>
       <c r="AB8" t="n">
         <v>0.440426087488492</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.454225572203327</v>
+        <v>0.454238441033183</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.306432576523578</v>
+        <v>0.306397646842541</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.215183380825444</v>
+        <v>0.215205441676625</v>
       </c>
       <c r="AF8" t="n">
         <v>0.0241584704476514</v>
@@ -1671,10 +1683,10 @@
         <v>41</v>
       </c>
       <c r="AH8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="AI8" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AJ8" t="s">
         <v>48</v>
@@ -1682,16 +1694,16 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E9" t="n">
         <v>40.338103</v>
@@ -1730,78 +1742,78 @@
         <v>0.144315431221174</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.337326791575047</v>
+        <v>0.337279387106885</v>
       </c>
       <c r="R9" t="n">
-        <v>0.503457697683629</v>
+        <v>0.503392011517538</v>
       </c>
       <c r="S9" t="n">
-        <v>0.176976952853648</v>
+        <v>0.176940990268175</v>
       </c>
       <c r="T9" t="n">
         <v>0.699098844689168</v>
       </c>
       <c r="U9" t="n">
-        <v>0.271158228524145</v>
+        <v>0.271125018360485</v>
       </c>
       <c r="V9" t="n">
-        <v>0.352080787415792</v>
+        <v>0.352053540623626</v>
       </c>
       <c r="W9" t="n">
-        <v>0.138672282484486</v>
+        <v>0.138644981242248</v>
       </c>
       <c r="X9" t="n">
         <v>0.0885204259288955</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.411348661233882</v>
+        <v>0.411415941941947</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.256781323698319</v>
+        <v>0.2568171399792</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.583010853746329</v>
+        <v>0.583052789313123</v>
       </c>
       <c r="AB9" t="n">
         <v>0.531001104610948</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.378281092012133</v>
+        <v>0.378141373287986</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.336115451787848</v>
+        <v>0.336323191469804</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.150273003033367</v>
+        <v>0.150204982075558</v>
       </c>
       <c r="AF9" t="n">
         <v>0.135330453166651</v>
       </c>
       <c r="AG9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="AH9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="AI9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="AJ9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D10" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E10" t="n">
         <v>40.358217</v>
@@ -1840,7 +1852,7 @@
         <v>0.138979491146434</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.399675374189391</v>
+        <v>0.399676731872367</v>
       </c>
       <c r="R10" t="n">
         <v>0.235995042348422</v>
@@ -1849,10 +1861,10 @@
         <v>0.535786135268456</v>
       </c>
       <c r="T10" t="n">
-        <v>0.703033398896009</v>
+        <v>0.703041014361947</v>
       </c>
       <c r="U10" t="n">
-        <v>0.280614319698918</v>
+        <v>0.280611488809424</v>
       </c>
       <c r="V10" t="n">
         <v>0.226152482983681</v>
@@ -1861,10 +1873,10 @@
         <v>0.405809793872041</v>
       </c>
       <c r="X10" t="n">
-        <v>0.0941110344513225</v>
+        <v>0.0941118852351122</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.349037439668319</v>
+        <v>0.349037917058714</v>
       </c>
       <c r="Z10" t="n">
         <v>0.52239978010311</v>
@@ -1873,10 +1885,10 @@
         <v>0.237294328597067</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.57185629168214</v>
+        <v>0.571863326111119</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.407535619082636</v>
+        <v>0.407541134295432</v>
       </c>
       <c r="AD10" t="n">
         <v>0.260185678830775</v>
@@ -1885,33 +1897,33 @@
         <v>0.185233936942734</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.147044765143855</v>
+        <v>0.14703924993106</v>
       </c>
       <c r="AG10" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="AH10" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="AI10" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="AJ10" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C11" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D11" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E11" t="n">
         <v>40.361706</v>
@@ -1953,49 +1965,49 @@
         <v>0.289248161493874</v>
       </c>
       <c r="R11" t="n">
-        <v>0.345392986534981</v>
+        <v>0.345406163537031</v>
       </c>
       <c r="S11" t="n">
-        <v>0.230527927078996</v>
+        <v>0.230531973387848</v>
       </c>
       <c r="T11" t="n">
-        <v>0.762098152774453</v>
+        <v>0.762114125868153</v>
       </c>
       <c r="U11" t="n">
         <v>0.524212924672261</v>
       </c>
       <c r="V11" t="n">
-        <v>0.351364960083831</v>
+        <v>0.351366380888303</v>
       </c>
       <c r="W11" t="n">
-        <v>0.370273211272706</v>
+        <v>0.370274083266828</v>
       </c>
       <c r="X11" t="n">
-        <v>0.153259323148316</v>
+        <v>0.153175016973061</v>
       </c>
       <c r="Y11" t="n">
         <v>0.244790018145876</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.216402155958678</v>
+        <v>0.216391224379916</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.4557501912365</v>
+        <v>0.455742507614012</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.378868476605154</v>
+        <v>0.378950540526822</v>
       </c>
       <c r="AC11" t="n">
         <v>0.359838220424671</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.322564573949812</v>
+        <v>0.322555381928486</v>
       </c>
       <c r="AE11" t="n">
-        <v>0.283496644912216</v>
+        <v>0.283515028954867</v>
       </c>
       <c r="AF11" t="n">
-        <v>0.0341005607133009</v>
+        <v>0.0340913686919754</v>
       </c>
       <c r="AG11" t="s">
         <v>40</v>
@@ -2004,670 +2016,890 @@
         <v>40</v>
       </c>
       <c r="AI11" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="AJ11" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B12" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C12" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D12" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="E12" t="n">
-        <v>40.38491</v>
+        <v>40.353131</v>
       </c>
       <c r="F12" t="n">
-        <v>-74.75798</v>
+        <v>-74.719621</v>
       </c>
       <c r="G12" t="n">
-        <v>40.394606</v>
+        <v>40.364018</v>
       </c>
       <c r="H12" t="n">
-        <v>-74.779177</v>
+        <v>-74.740553</v>
       </c>
       <c r="I12" t="n">
-        <v>40.375683</v>
+        <v>40.343789</v>
       </c>
       <c r="J12" t="n">
-        <v>-74.736848</v>
+        <v>-74.698588</v>
       </c>
       <c r="K12" t="n">
-        <v>0.297101449275362</v>
+        <v>0.303571428571429</v>
       </c>
       <c r="L12" t="n">
-        <v>0.136866232854076</v>
+        <v>0.131435681939588</v>
       </c>
       <c r="M12" t="n">
-        <v>0.329545454545455</v>
+        <v>0.4</v>
       </c>
       <c r="N12" t="n">
-        <v>0.142902697863645</v>
+        <v>0.121094983674709</v>
       </c>
       <c r="O12" t="n">
-        <v>0.380392156862745</v>
+        <v>0.282352941176471</v>
       </c>
       <c r="P12" t="n">
-        <v>0.169647235699781</v>
+        <v>0.136066457164305</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.325393569159018</v>
+        <v>0.381065086319017</v>
       </c>
       <c r="R12" t="n">
-        <v>0.202048929206734</v>
+        <v>0.281900773753168</v>
       </c>
       <c r="S12" t="n">
-        <v>0.558025693418098</v>
+        <v>0.190749968110651</v>
       </c>
       <c r="T12" t="n">
-        <v>0.590848472137417</v>
+        <v>0.774518977325699</v>
       </c>
       <c r="U12" t="n">
-        <v>0.385276069448176</v>
+        <v>0.373610088479064</v>
       </c>
       <c r="V12" t="n">
-        <v>0.229039577238636</v>
+        <v>0.468612830033711</v>
       </c>
       <c r="W12" t="n">
-        <v>0.534493742518764</v>
+        <v>0.255512004701204</v>
       </c>
       <c r="X12" t="n">
-        <v>0.126235064768519</v>
+        <v>0.112129471519306</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.311205972216737</v>
+        <v>0.189476533671468</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.55639168863251</v>
+        <v>0.345154349228878</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.120862340052599</v>
+        <v>0.464939795894354</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.419156170374463</v>
+        <v>0.447493271223103</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.493390936666973</v>
+        <v>0.420796029046787</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.359678279253608</v>
+        <v>0.40573030609431</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.0850795109844655</v>
+        <v>0.137861935839691</v>
       </c>
       <c r="AF12" t="n">
-        <v>0.0618512730949536</v>
+        <v>0.0356117290192113</v>
       </c>
       <c r="AG12" t="s">
-        <v>104</v>
+        <v>47</v>
       </c>
       <c r="AH12" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="AI12" t="s">
-        <v>105</v>
+        <v>57</v>
       </c>
       <c r="AJ12" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C13" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D13" t="s">
         <v>103</v>
       </c>
       <c r="E13" t="n">
-        <v>40.328281</v>
+        <v>40.38491</v>
       </c>
       <c r="F13" t="n">
-        <v>-74.804559</v>
+        <v>-74.75798</v>
       </c>
       <c r="G13" t="n">
-        <v>40.33784</v>
+        <v>40.394606</v>
       </c>
       <c r="H13" t="n">
-        <v>-74.825575</v>
+        <v>-74.779177</v>
       </c>
       <c r="I13" t="n">
-        <v>40.319148</v>
+        <v>40.375683</v>
       </c>
       <c r="J13" t="n">
-        <v>-74.783438</v>
+        <v>-74.736848</v>
       </c>
       <c r="K13" t="n">
-        <v>0.300925925925926</v>
+        <v>0.297101449275362</v>
       </c>
       <c r="L13" t="n">
-        <v>0.146281186801123</v>
+        <v>0.136866232854076</v>
       </c>
       <c r="M13" t="n">
-        <v>0.328358208955224</v>
+        <v>0.329545454545455</v>
       </c>
       <c r="N13" t="n">
-        <v>0.145679208548386</v>
+        <v>0.142902697863645</v>
       </c>
       <c r="O13" t="n">
-        <v>0.364705882352941</v>
+        <v>0.380392156862745</v>
       </c>
       <c r="P13" t="n">
-        <v>0.137882238499753</v>
+        <v>0.169647235699781</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.29882428487279</v>
+        <v>0.325393569159018</v>
       </c>
       <c r="R13" t="n">
-        <v>0.157559664937524</v>
+        <v>0.202048929206734</v>
       </c>
       <c r="S13" t="n">
-        <v>0.430997275471134</v>
+        <v>0.558025693418098</v>
       </c>
       <c r="T13" t="n">
-        <v>0.63872132224914</v>
+        <v>0.590848472137417</v>
       </c>
       <c r="U13" t="n">
-        <v>0.35122693863842</v>
+        <v>0.385276069448176</v>
       </c>
       <c r="V13" t="n">
-        <v>0.217829860403129</v>
+        <v>0.229039577238636</v>
       </c>
       <c r="W13" t="n">
-        <v>0.478118420244124</v>
+        <v>0.534493742518764</v>
       </c>
       <c r="X13" t="n">
-        <v>0.0827147002890197</v>
+        <v>0.126235064768519</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.346179528457546</v>
+        <v>0.311205972216737</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.495623768608962</v>
+        <v>0.55639168863251</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.18889976021098</v>
+        <v>0.120862340052599</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.474337272987963</v>
+        <v>0.419156170374463</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.405871863222723</v>
+        <v>0.493390936666973</v>
       </c>
       <c r="AD13" t="n">
-        <v>0.295131905506021</v>
+        <v>0.359678279253608</v>
       </c>
       <c r="AE13" t="n">
-        <v>0.23840610350216</v>
+        <v>0.0850795109844655</v>
       </c>
       <c r="AF13" t="n">
-        <v>0.0605901277690964</v>
+        <v>0.0618512730949536</v>
       </c>
       <c r="AG13" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="AH13" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="AI13" t="s">
-        <v>47</v>
+        <v>105</v>
       </c>
       <c r="AJ13" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B14" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D14" t="s">
         <v>103</v>
       </c>
       <c r="E14" t="n">
-        <v>40.321026</v>
+        <v>40.328281</v>
       </c>
       <c r="F14" t="n">
-        <v>-74.78868</v>
+        <v>-74.804559</v>
       </c>
       <c r="G14" t="n">
-        <v>40.330632</v>
+        <v>40.33784</v>
       </c>
       <c r="H14" t="n">
-        <v>-74.809579</v>
+        <v>-74.825575</v>
       </c>
       <c r="I14" t="n">
-        <v>40.311546</v>
+        <v>40.319148</v>
       </c>
       <c r="J14" t="n">
-        <v>-74.767619</v>
+        <v>-74.783438</v>
       </c>
       <c r="K14" t="n">
-        <v>0.323529411764706</v>
+        <v>0.300925925925926</v>
       </c>
       <c r="L14" t="n">
-        <v>0.142138345533739</v>
+        <v>0.146281186801123</v>
       </c>
       <c r="M14" t="n">
-        <v>0.35</v>
+        <v>0.328358208955224</v>
       </c>
       <c r="N14" t="n">
-        <v>0.144639523172478</v>
+        <v>0.145679208548386</v>
       </c>
       <c r="O14" t="n">
-        <v>0.345098039215686</v>
+        <v>0.364705882352941</v>
       </c>
       <c r="P14" t="n">
-        <v>0.135458622877551</v>
+        <v>0.137882238499753</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.292092629808491</v>
+        <v>0.29882428487279</v>
       </c>
       <c r="R14" t="n">
-        <v>0.428311847479398</v>
+        <v>0.157559664937524</v>
       </c>
       <c r="S14" t="n">
-        <v>0.155937391541153</v>
+        <v>0.430997275471134</v>
       </c>
       <c r="T14" t="n">
-        <v>0.661641591481738</v>
+        <v>0.63872132224914</v>
       </c>
       <c r="U14" t="n">
-        <v>0.34742573031661</v>
+        <v>0.35122693863842</v>
       </c>
       <c r="V14" t="n">
-        <v>0.456895667451419</v>
+        <v>0.217829860403129</v>
       </c>
       <c r="W14" t="n">
-        <v>0.189500164328434</v>
+        <v>0.478118420244124</v>
       </c>
       <c r="X14" t="n">
-        <v>0.0812793185071385</v>
+        <v>0.0827147002890197</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.372266338700046</v>
+        <v>0.346179528457546</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.20256911429179</v>
+        <v>0.495623768608962</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.510294841833704</v>
+        <v>0.18889976021098</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.481926044610384</v>
+        <v>0.474337272987963</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.447030057909734</v>
+        <v>0.405871863222723</v>
       </c>
       <c r="AD14" t="n">
-        <v>0.309943928669914</v>
+        <v>0.295131905506021</v>
       </c>
       <c r="AE14" t="n">
-        <v>0.184171339277507</v>
+        <v>0.23840610350216</v>
       </c>
       <c r="AF14" t="n">
-        <v>0.058854674142844</v>
+        <v>0.0605901277690964</v>
       </c>
       <c r="AG14" t="s">
-        <v>41</v>
+        <v>109</v>
       </c>
       <c r="AH14" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="AI14" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="AJ14" t="s">
-        <v>114</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C15" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D15" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="E15" t="n">
-        <v>40.343974</v>
+        <v>40.321026</v>
       </c>
       <c r="F15" t="n">
-        <v>-74.656639</v>
+        <v>-74.78868</v>
       </c>
       <c r="G15" t="n">
-        <v>40.354959</v>
+        <v>40.330632</v>
       </c>
       <c r="H15" t="n">
-        <v>-74.677713</v>
+        <v>-74.809579</v>
       </c>
       <c r="I15" t="n">
-        <v>40.334793</v>
+        <v>40.311546</v>
       </c>
       <c r="J15" t="n">
-        <v>-74.635716</v>
+        <v>-74.767619</v>
       </c>
       <c r="K15" t="n">
-        <v>0.40625</v>
+        <v>0.323529411764706</v>
       </c>
       <c r="L15" t="n">
-        <v>0.184562387891951</v>
+        <v>0.142138345533739</v>
       </c>
       <c r="M15" t="n">
-        <v>0.240963855421687</v>
+        <v>0.35</v>
       </c>
       <c r="N15" t="n">
-        <v>0.125843603932378</v>
+        <v>0.144639523172478</v>
       </c>
       <c r="O15" t="n">
-        <v>0.396078431372549</v>
+        <v>0.345098039215686</v>
       </c>
       <c r="P15" t="n">
-        <v>0.143864437924161</v>
+        <v>0.135458622877551</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.35113171535896</v>
+        <v>0.292080375933529</v>
       </c>
       <c r="R15" t="n">
-        <v>0.525861625511708</v>
+        <v>0.428311830437071</v>
       </c>
       <c r="S15" t="n">
-        <v>0.698246073912356</v>
+        <v>0.15592231129015</v>
       </c>
       <c r="T15" t="n">
-        <v>0.190883098215235</v>
+        <v>0.661641591481738</v>
       </c>
       <c r="U15" t="n">
-        <v>0.262755980033652</v>
+        <v>0.347413671474267</v>
       </c>
       <c r="V15" t="n">
-        <v>0.352370537350509</v>
+        <v>0.456895489929101</v>
       </c>
       <c r="W15" t="n">
-        <v>0.0896759343068521</v>
+        <v>0.189478191521914</v>
       </c>
       <c r="X15" t="n">
-        <v>0.136693027367445</v>
+        <v>0.0812793185071385</v>
       </c>
       <c r="Y15" t="n">
-        <v>0.398596012705191</v>
+        <v>0.37227171221953</v>
       </c>
       <c r="Z15" t="n">
-        <v>0.255840011867245</v>
+        <v>0.20256998294444</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.541934707519162</v>
+        <v>0.510326129093632</v>
       </c>
       <c r="AB15" t="n">
-        <v>0.572153035585578</v>
+        <v>0.481926044610384</v>
       </c>
       <c r="AC15" t="n">
-        <v>0.386324110671937</v>
+        <v>0.447087048441952</v>
       </c>
       <c r="AD15" t="n">
-        <v>0.28188252596746</v>
+        <v>0.30994576707418</v>
       </c>
       <c r="AE15" t="n">
-        <v>0.167153230995496</v>
+        <v>0.184112510341024</v>
       </c>
       <c r="AF15" t="n">
-        <v>0.164640132365107</v>
+        <v>0.058854674142844</v>
       </c>
       <c r="AG15" t="s">
-        <v>119</v>
+        <v>41</v>
       </c>
       <c r="AH15" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="AI15" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="AJ15" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B16" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C16" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D16" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" t="n">
+        <v>40.343974</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-74.656639</v>
+      </c>
+      <c r="G16" t="n">
+        <v>40.354959</v>
+      </c>
+      <c r="H16" t="n">
+        <v>-74.677713</v>
+      </c>
+      <c r="I16" t="n">
+        <v>40.334793</v>
+      </c>
+      <c r="J16" t="n">
+        <v>-74.635716</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.40625</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.184562387891951</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.240963855421687</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.125843603932378</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.396078431372549</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.143864437924161</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.352207980668438</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.526835335537456</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0.698224033500604</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0.191998457585878</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0.26328172433716</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0.353221239230179</v>
+      </c>
+      <c r="W16" t="n">
+        <v>0.0897349438459205</v>
+      </c>
+      <c r="X16" t="n">
+        <v>0.137518130396542</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>0.397335212932007</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>0.255244653529876</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>0.541730667585445</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>0.571119115312381</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>0.387397738762754</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>0.278558691056163</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>0.167292949719643</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>0.166750620461439</v>
+      </c>
+      <c r="AG16" t="s">
         <v>118</v>
       </c>
-      <c r="E16" t="n">
-        <v>40.342717</v>
-      </c>
-      <c r="F16" t="n">
-        <v>-74.650305</v>
-      </c>
-      <c r="G16" t="n">
-        <v>40.353617</v>
-      </c>
-      <c r="H16" t="n">
-        <v>-74.671335</v>
-      </c>
-      <c r="I16" t="n">
-        <v>40.333492</v>
-      </c>
-      <c r="J16" t="n">
-        <v>-74.629285</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0.401234567901235</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0.190442775284621</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0.239583333333333</v>
-      </c>
-      <c r="N16" t="n">
-        <v>0.127703309174295</v>
-      </c>
-      <c r="O16" t="n">
-        <v>0.407843137254902</v>
-      </c>
-      <c r="P16" t="n">
-        <v>0.144644469374759</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>0.339678597503287</v>
-      </c>
-      <c r="R16" t="n">
-        <v>0.530503122548382</v>
-      </c>
-      <c r="S16" t="n">
-        <v>0.702316626659081</v>
-      </c>
-      <c r="T16" t="n">
-        <v>0.178548136532459</v>
-      </c>
-      <c r="U16" t="n">
-        <v>0.263108358935227</v>
-      </c>
-      <c r="V16" t="n">
-        <v>0.346706682755228</v>
-      </c>
-      <c r="W16" t="n">
-        <v>0.0876216733096653</v>
-      </c>
-      <c r="X16" t="n">
-        <v>0.132104272194292</v>
-      </c>
-      <c r="Y16" t="n">
-        <v>0.416056768856574</v>
-      </c>
-      <c r="Z16" t="n">
-        <v>0.262624238844213</v>
-      </c>
-      <c r="AA16" t="n">
-        <v>0.547597315165699</v>
-      </c>
-      <c r="AB16" t="n">
-        <v>0.587436409106286</v>
-      </c>
-      <c r="AC16" t="n">
-        <v>0.381862303520544</v>
-      </c>
-      <c r="AD16" t="n">
-        <v>0.294379998161596</v>
-      </c>
-      <c r="AE16" t="n">
-        <v>0.164540858534792</v>
-      </c>
-      <c r="AF16" t="n">
-        <v>0.159216839783068</v>
-      </c>
-      <c r="AG16" t="s">
-        <v>84</v>
-      </c>
       <c r="AH16" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="AI16" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="AJ16" t="s">
-        <v>86</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" t="n">
+        <v>40.342717</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-74.650305</v>
+      </c>
+      <c r="G17" t="n">
+        <v>40.353617</v>
+      </c>
+      <c r="H17" t="n">
+        <v>-74.671335</v>
+      </c>
+      <c r="I17" t="n">
+        <v>40.333492</v>
+      </c>
+      <c r="J17" t="n">
+        <v>-74.629285</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.401234567901235</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.190442775284621</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.239583333333333</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.127703309174295</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.407843137254902</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.144644469374759</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.339031832334921</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.52958372822167</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.702315576925458</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0.177921169342105</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0.262604386419732</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0.346428783569233</v>
+      </c>
+      <c r="W17" t="n">
+        <v>0.0876092333192684</v>
+      </c>
+      <c r="X17" t="n">
+        <v>0.131672441686606</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>0.416845703855392</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>0.263114292064012</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>0.547609883320447</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>0.588084725952029</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>0.380751907344425</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>0.296661457854582</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>0.164529828109201</v>
+      </c>
+      <c r="AF17" t="n">
+        <v>0.158056806691792</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>104</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>123</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
         <v>124</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>125</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>126</v>
       </c>
-      <c r="D17" t="s">
-        <v>118</v>
-      </c>
-      <c r="E17" t="n">
+      <c r="D18" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" t="n">
+        <v>40.345588</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-74.654241</v>
+      </c>
+      <c r="G18" t="n">
+        <v>40.356659</v>
+      </c>
+      <c r="H18" t="n">
+        <v>-74.675203</v>
+      </c>
+      <c r="I18" t="n">
+        <v>40.336579</v>
+      </c>
+      <c r="J18" t="n">
+        <v>-74.633262</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.41358024691358</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.1847427930511</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.238095238095238</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.128961304652451</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.396078431372549</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.141867623839505</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.36275445808786</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.541023369448056</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0.209632175764592</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0.699444544294824</v>
+      </c>
+      <c r="U18" t="n">
+        <v>0.267450098007967</v>
+      </c>
+      <c r="V18" t="n">
+        <v>0.356711114587473</v>
+      </c>
+      <c r="W18" t="n">
+        <v>0.141966096914688</v>
+      </c>
+      <c r="X18" t="n">
+        <v>0.0898061488971261</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>0.387835839057397</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>0.253297003327624</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>0.552991891505294</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>0.547300703316466</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>0.376069491681221</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>0.26722309035757</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>0.182954315654012</v>
+      </c>
+      <c r="AF18" t="n">
+        <v>0.173753102307197</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>81</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>119</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" t="s">
+        <v>130</v>
+      </c>
+      <c r="D19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" t="n">
         <v>40.334348</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F19" t="n">
         <v>-74.647146</v>
       </c>
-      <c r="G17" t="n">
+      <c r="G19" t="n">
         <v>40.345334</v>
       </c>
-      <c r="H17" t="n">
+      <c r="H19" t="n">
         <v>-74.668232</v>
       </c>
-      <c r="I17" t="n">
+      <c r="I19" t="n">
         <v>40.325165</v>
       </c>
-      <c r="J17" t="n">
+      <c r="J19" t="n">
         <v>-74.626075</v>
       </c>
-      <c r="K17" t="n">
+      <c r="K19" t="n">
         <v>0.397849462365591</v>
       </c>
-      <c r="L17" t="n">
+      <c r="L19" t="n">
         <v>0.185525355726783</v>
       </c>
-      <c r="M17" t="n">
+      <c r="M19" t="n">
         <v>0.256410256410256</v>
       </c>
-      <c r="N17" t="n">
+      <c r="N19" t="n">
         <v>0.126551194230143</v>
       </c>
-      <c r="O17" t="n">
+      <c r="O19" t="n">
         <v>0.403921568627451</v>
       </c>
-      <c r="P17" t="n">
+      <c r="P19" t="n">
         <v>0.14517297296093</v>
       </c>
-      <c r="Q17" t="n">
-        <v>0.501059510184396</v>
-      </c>
-      <c r="R17" t="n">
-        <v>0.326743136334162</v>
-      </c>
-      <c r="S17" t="n">
+      <c r="Q19" t="n">
+        <v>0.501073712888876</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0.32674098177454</v>
+      </c>
+      <c r="S19" t="n">
         <v>0.163123215176832</v>
       </c>
-      <c r="T17" t="n">
-        <v>0.708631664241287</v>
-      </c>
-      <c r="U17" t="n">
-        <v>0.347916147550062</v>
-      </c>
-      <c r="V17" t="n">
-        <v>0.267123264763407</v>
-      </c>
-      <c r="W17" t="n">
+      <c r="T19" t="n">
+        <v>0.708645208321089</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0.347887624441874</v>
+      </c>
+      <c r="V19" t="n">
+        <v>0.267131916124209</v>
+      </c>
+      <c r="W19" t="n">
         <v>0.133304387082807</v>
       </c>
-      <c r="X17" t="n">
-        <v>0.0827013893129456</v>
-      </c>
-      <c r="Y17" t="n">
-        <v>0.271166828384603</v>
-      </c>
-      <c r="Z17" t="n">
-        <v>0.434737469188166</v>
-      </c>
-      <c r="AA17" t="n">
+      <c r="X19" t="n">
+        <v>0.0826916764915203</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>0.271162351512836</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>0.434743938732916</v>
+      </c>
+      <c r="AA19" t="n">
         <v>0.599291630794096</v>
       </c>
-      <c r="AB17" t="n">
-        <v>0.545369178617046</v>
-      </c>
-      <c r="AC17" t="n">
-        <v>0.35530471550694</v>
-      </c>
-      <c r="AD17" t="n">
-        <v>0.351982718999908</v>
-      </c>
-      <c r="AE17" t="n">
+      <c r="AB19" t="n">
+        <v>0.545428189568998</v>
+      </c>
+      <c r="AC19" t="n">
+        <v>0.355337806783712</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>0.351980880595643</v>
+      </c>
+      <c r="AE19" t="n">
         <v>0.15399577167019</v>
       </c>
-      <c r="AF17" t="n">
-        <v>0.138716793822962</v>
-      </c>
-      <c r="AG17" t="s">
-        <v>64</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>127</v>
-      </c>
-      <c r="AI17" t="s">
-        <v>128</v>
-      </c>
-      <c r="AJ17" t="s">
-        <v>74</v>
+      <c r="AF19" t="n">
+        <v>0.138685540950455</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>131</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>132</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2686,10 +2918,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2">
@@ -2697,7 +2929,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3">
@@ -2705,7 +2937,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4">
@@ -2713,7 +2945,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5">
@@ -2721,7 +2953,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6">
@@ -2729,7 +2961,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7">
@@ -2737,7 +2969,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8">
@@ -2745,7 +2977,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9">
@@ -2753,7 +2985,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10">
@@ -2761,7 +2993,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11">
@@ -2769,7 +3001,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12">
@@ -2777,7 +3009,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13">
@@ -2785,7 +3017,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14">
@@ -2793,7 +3025,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15">
@@ -2801,7 +3033,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16">
@@ -2809,7 +3041,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17">
@@ -2817,7 +3049,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18">
@@ -2825,7 +3057,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19">
@@ -2833,7 +3065,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20">
@@ -2841,7 +3073,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21">
@@ -2849,7 +3081,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22">
@@ -2857,7 +3089,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23">
@@ -2865,7 +3097,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24">
@@ -2873,7 +3105,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25">
@@ -2881,7 +3113,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26">
@@ -2889,7 +3121,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27">
@@ -2897,7 +3129,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="28">
@@ -2905,7 +3137,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29">
@@ -2913,7 +3145,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30">
@@ -2921,7 +3153,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31">
@@ -2929,7 +3161,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32">
@@ -2937,7 +3169,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33">
@@ -2945,7 +3177,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34">
@@ -2953,7 +3185,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35">
@@ -2961,7 +3193,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36">
@@ -2969,7 +3201,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37">
@@ -2977,7 +3209,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated data files to include princeton public library
</commit_message>
<xml_diff>
--- a/datasets/satelliteData/satHsvFinal4.xlsx
+++ b/datasets/satelliteData/satHsvFinal4.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="160">
   <si>
     <t xml:space="preserve">sat_label</t>
   </si>
@@ -156,153 +156,159 @@
     <t xml:space="preserve">Double Brook Farm; Bayberry</t>
   </si>
   <si>
+    <t xml:space="preserve">gray23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">farmLawrenceville</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/farmLawrenceville.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lawrenceville School’s Big Red Farm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">farmStony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/farmStony.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stony Ford Field Station Farm</t>
+  </si>
+  <si>
     <t xml:space="preserve">gray15</t>
   </si>
   <si>
+    <t xml:space="preserve">gray26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gardenMtLake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/gardenMtLake.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mt. Lake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">garden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">darkslategray</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gardenPrinceton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/gardenPrinceton.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Princeton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cornsilk4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">golfHopewell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/golfHopewell.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hopewell Golf course</t>
+  </si>
+  <si>
+    <t xml:space="preserve">golf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lemonchiffon4</t>
+  </si>
+  <si>
     <t xml:space="preserve">dimgray</t>
   </si>
   <si>
-    <t xml:space="preserve">gray40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">farmLawrenceville</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/farmLawrenceville.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lawrenceville School’s Big Red Farm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">farmStony</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/farmStony.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stony Ford Field Station Farm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gardenMtLake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/gardenMtLake.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mt. Lake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">garden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">darkslategray</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gardenPrinceton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/gardenPrinceton.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Princeton</t>
+    <t xml:space="preserve">golfPrinceton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/golfPrinceton.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Princeton golf course</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ivory4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preserveMtLakes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/preserveMtLakes.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billie Johnson Mountain Lakes Nature Preserve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preserve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preserveMtRose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/preserveMtRose.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mt Rose Preserve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray14</t>
   </si>
   <si>
     <t xml:space="preserve">gray31</t>
   </si>
   <si>
-    <t xml:space="preserve">gray20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lemonchiffon4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">golfHopewell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/golfHopewell.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hopewell Golf course</t>
-  </si>
-  <si>
-    <t xml:space="preserve">golf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">golfPrinceton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/golfPrinceton.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Princeton golf course</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ivory4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preserveMtLakes1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/preserveMtLakes1000.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billie Johnson Mountain Lakes Nature Preserve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preserve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">darkseagreen4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preserveMtRose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/preserveMtRose.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mt Rose Preserve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">darkolivegreen4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray35</t>
-  </si>
-  <si>
     <t xml:space="preserve">preserveStonyOctagon</t>
   </si>
   <si>
@@ -327,9 +333,6 @@
     <t xml:space="preserve">school</t>
   </si>
   <si>
-    <t xml:space="preserve">gray23</t>
-  </si>
-  <si>
     <t xml:space="preserve">gray9</t>
   </si>
   <si>
@@ -384,9 +387,6 @@
     <t xml:space="preserve">Forest; SW Track and Jadwin Gym; Princeton Univ</t>
   </si>
   <si>
-    <t xml:space="preserve">gray52</t>
-  </si>
-  <si>
     <t xml:space="preserve">univGuyotHall</t>
   </si>
   <si>
@@ -396,9 +396,6 @@
     <t xml:space="preserve">Guyot Hall; Princeton Univ</t>
   </si>
   <si>
-    <t xml:space="preserve">gray32</t>
-  </si>
-  <si>
     <t xml:space="preserve">univSolarFarm</t>
   </si>
   <si>
@@ -412,6 +409,21 @@
   </si>
   <si>
     <t xml:space="preserve">gray57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">urbanLibrary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/urbanLibrary.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Princeton Public Library</t>
+  </si>
+  <si>
+    <t xml:space="preserve">urban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">azure4</t>
   </si>
   <si>
     <t xml:space="preserve">variableName</t>
@@ -1082,75 +1094,75 @@
         <v>0.136411781841319</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.348399319418516</v>
+        <v>0.286427215361963</v>
       </c>
       <c r="R3" t="n">
-        <v>0.27784732799299</v>
+        <v>0.362889726704319</v>
       </c>
       <c r="S3" t="n">
-        <v>0.19267140628594</v>
+        <v>0.205916542451176</v>
       </c>
       <c r="T3" t="n">
-        <v>0.768234550270837</v>
+        <v>0.776810086765093</v>
       </c>
       <c r="U3" t="n">
-        <v>0.402966035288512</v>
+        <v>0.489979056547318</v>
       </c>
       <c r="V3" t="n">
-        <v>0.463101953310469</v>
+        <v>0.366378275528389</v>
       </c>
       <c r="W3" t="n">
-        <v>0.248102325074812</v>
+        <v>0.290757042677842</v>
       </c>
       <c r="X3" t="n">
-        <v>0.122429261787393</v>
+        <v>0.117100439652045</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.197951740525308</v>
+        <v>0.323367216093884</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.378367451507324</v>
+        <v>0.199749393185288</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.456042444462877</v>
+        <v>0.45862202728189</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.429280782048271</v>
+        <v>0.442426791480877</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.438251677543892</v>
+        <v>0.382038790329994</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.354431473481018</v>
+        <v>0.35539847412446</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.167219413549039</v>
+        <v>0.224509605662285</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.0400974354260502</v>
+        <v>0.0380531298832613</v>
       </c>
       <c r="AG3" t="s">
         <v>47</v>
       </c>
       <c r="AH3" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="AI3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AJ3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
         <v>39</v>
@@ -1246,21 +1258,21 @@
         <v>41</v>
       </c>
       <c r="AI4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AJ4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
         <v>39</v>
@@ -1302,78 +1314,78 @@
         <v>0.136279722924118</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.37961453231836</v>
+        <v>0.379734376620002</v>
       </c>
       <c r="R5" t="n">
-        <v>0.280721337264827</v>
+        <v>0.280779349365682</v>
       </c>
       <c r="S5" t="n">
-        <v>0.187757607754354</v>
+        <v>0.187858675071881</v>
       </c>
       <c r="T5" t="n">
-        <v>0.775034535247682</v>
+        <v>0.775050840819737</v>
       </c>
       <c r="U5" t="n">
-        <v>0.375586942757632</v>
+        <v>0.375429326599417</v>
       </c>
       <c r="V5" t="n">
-        <v>0.466275393892707</v>
+        <v>0.466365749127651</v>
       </c>
       <c r="W5" t="n">
-        <v>0.250026745501884</v>
+        <v>0.25028820553429</v>
       </c>
       <c r="X5" t="n">
-        <v>0.112384389496513</v>
+        <v>0.112375368584235</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.189560197910951</v>
+        <v>0.189535249712218</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.351171178127506</v>
+        <v>0.350888410212513</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.465924329403919</v>
+        <v>0.465868934884591</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.446826682492629</v>
+        <v>0.446852499558382</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.428826178876735</v>
+        <v>0.428210313447927</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.403349572571008</v>
+        <v>0.403689677360051</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.1321095688942</v>
+        <v>0.132389006342495</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.0357146796580568</v>
+        <v>0.0357110028495266</v>
       </c>
       <c r="AG5" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="AH5" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="AI5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="AJ5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E6" t="n">
         <v>40.365934</v>
@@ -1412,78 +1424,78 @@
         <v>0.135161968799217</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.362383872521582</v>
+        <v>0.362378031017664</v>
       </c>
       <c r="R6" t="n">
-        <v>0.500389745714076</v>
+        <v>0.500370779355212</v>
       </c>
       <c r="S6" t="n">
-        <v>0.240184213816329</v>
+        <v>0.240178135255276</v>
       </c>
       <c r="T6" t="n">
         <v>0.687650725398028</v>
       </c>
       <c r="U6" t="n">
-        <v>0.319270292188147</v>
+        <v>0.319258964610822</v>
       </c>
       <c r="V6" t="n">
-        <v>0.38729163908905</v>
+        <v>0.387294412924983</v>
       </c>
       <c r="W6" t="n">
-        <v>0.181111585767093</v>
+        <v>0.181108538341975</v>
       </c>
       <c r="X6" t="n">
         <v>0.0958285240958132</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.353415612746418</v>
+        <v>0.353423647100445</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.220703335260754</v>
+        <v>0.220718759573085</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.517280857042752</v>
+        <v>0.51728731497723</v>
       </c>
       <c r="AB6" t="n">
         <v>0.546007421579363</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.476326868278334</v>
+        <v>0.476284584980237</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.261647210221528</v>
+        <v>0.261700523945216</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.157909734350584</v>
+        <v>0.157898703924993</v>
       </c>
       <c r="AF6" t="n">
         <v>0.104116187149554</v>
       </c>
       <c r="AG6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AH6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="AI6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="AJ6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E7" t="n">
         <v>40.347059</v>
@@ -1522,78 +1534,78 @@
         <v>0.141336961844477</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.378449003640395</v>
+        <v>0.368804034382226</v>
       </c>
       <c r="R7" t="n">
-        <v>0.542971395077246</v>
+        <v>0.540333760598456</v>
       </c>
       <c r="S7" t="n">
-        <v>0.225363593168575</v>
+        <v>0.221063536378446</v>
       </c>
       <c r="T7" t="n">
-        <v>0.699342372843117</v>
+        <v>0.698919899052576</v>
       </c>
       <c r="U7" t="n">
-        <v>0.271980705841052</v>
+        <v>0.271197822819021</v>
       </c>
       <c r="V7" t="n">
-        <v>0.374500758063418</v>
+        <v>0.363194527338301</v>
       </c>
       <c r="W7" t="n">
-        <v>0.153632979216308</v>
+        <v>0.148692061374659</v>
       </c>
       <c r="X7" t="n">
-        <v>0.0925204579492771</v>
+        <v>0.0912785914911102</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.370722435119189</v>
+        <v>0.378736424153979</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.244852292294164</v>
+        <v>0.249394561470606</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.538342980372586</v>
+        <v>0.542303778243217</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.543221886331469</v>
+        <v>0.546325179070443</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.388272819192941</v>
+        <v>0.377781046052027</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.228460336427981</v>
+        <v>0.253120691240004</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.206335141097527</v>
+        <v>0.194288077948341</v>
       </c>
       <c r="AF7" t="n">
-        <v>0.176931703281552</v>
+        <v>0.174810184759629</v>
       </c>
       <c r="AG7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="AH7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="AI7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="AJ7" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E8" t="n">
         <v>40.364166</v>
@@ -1632,78 +1644,78 @@
         <v>0.137237314427854</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.301448007786584</v>
+        <v>0.300817422346192</v>
       </c>
       <c r="R8" t="n">
-        <v>0.404124568183147</v>
+        <v>0.403443951047723</v>
       </c>
       <c r="S8" t="n">
-        <v>0.169684550278726</v>
+        <v>0.169393051939012</v>
       </c>
       <c r="T8" t="n">
-        <v>0.660106479673258</v>
+        <v>0.660088596444441</v>
       </c>
       <c r="U8" t="n">
-        <v>0.36232169399861</v>
+        <v>0.362221215211254</v>
       </c>
       <c r="V8" t="n">
-        <v>0.427698684951855</v>
+        <v>0.426820740337222</v>
       </c>
       <c r="W8" t="n">
-        <v>0.217352690291093</v>
+        <v>0.216890739940572</v>
       </c>
       <c r="X8" t="n">
-        <v>0.0930083757348977</v>
+        <v>0.0930267294682656</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.375694172149662</v>
+        <v>0.376830177221663</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.210050829920029</v>
+        <v>0.210931973601705</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.528062208558599</v>
+        <v>0.528304069001079</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.440426087488492</v>
+        <v>0.440400839632818</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.454238441033183</v>
+        <v>0.451144406655023</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.306397646842541</v>
+        <v>0.31051199558783</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.215205441676625</v>
+        <v>0.214181450500965</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.0241584704476514</v>
+        <v>0.0241621472561816</v>
       </c>
       <c r="AG8" t="s">
         <v>41</v>
       </c>
       <c r="AH8" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="AI8" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="AJ8" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" t="s">
         <v>78</v>
-      </c>
-      <c r="C9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" t="s">
-        <v>75</v>
       </c>
       <c r="E9" t="n">
         <v>40.338103</v>
@@ -1742,78 +1754,78 @@
         <v>0.144315431221174</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.337279387106885</v>
+        <v>0.337326791575047</v>
       </c>
       <c r="R9" t="n">
-        <v>0.503392011517538</v>
+        <v>0.503457697683629</v>
       </c>
       <c r="S9" t="n">
-        <v>0.176940990268175</v>
+        <v>0.176976952853648</v>
       </c>
       <c r="T9" t="n">
         <v>0.699098844689168</v>
       </c>
       <c r="U9" t="n">
-        <v>0.271125018360485</v>
+        <v>0.271158228524145</v>
       </c>
       <c r="V9" t="n">
-        <v>0.352053540623626</v>
+        <v>0.352080787415792</v>
       </c>
       <c r="W9" t="n">
-        <v>0.138644981242248</v>
+        <v>0.138672282484486</v>
       </c>
       <c r="X9" t="n">
         <v>0.0885204259288955</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.411415941941947</v>
+        <v>0.411348661233882</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.2568171399792</v>
+        <v>0.256781323698319</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.583052789313123</v>
+        <v>0.583010853746329</v>
       </c>
       <c r="AB9" t="n">
         <v>0.531001104610948</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.378141373287986</v>
+        <v>0.378281092012133</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.336323191469804</v>
+        <v>0.336115451787848</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.150204982075558</v>
+        <v>0.150273003033367</v>
       </c>
       <c r="AF9" t="n">
         <v>0.135330453166651</v>
       </c>
       <c r="AG9" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AH9" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="AI9" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="AJ9" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D10" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E10" t="n">
         <v>40.358217</v>
@@ -1837,93 +1849,93 @@
         <v>0.4</v>
       </c>
       <c r="L10" t="n">
-        <v>0.174636112149688</v>
+        <v>0.166777836747658</v>
       </c>
       <c r="M10" t="n">
-        <v>0.279411764705882</v>
+        <v>0.28</v>
       </c>
       <c r="N10" t="n">
-        <v>0.124759789714527</v>
+        <v>0.125462894106281</v>
       </c>
       <c r="O10" t="n">
-        <v>0.388235294117647</v>
+        <v>0.372549019607843</v>
       </c>
       <c r="P10" t="n">
-        <v>0.138979491146434</v>
+        <v>0.142659818227208</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.399676731872367</v>
+        <v>0.355995495087241</v>
       </c>
       <c r="R10" t="n">
-        <v>0.235995042348422</v>
+        <v>0.504603935424321</v>
       </c>
       <c r="S10" t="n">
-        <v>0.535786135268456</v>
+        <v>0.235661504480482</v>
       </c>
       <c r="T10" t="n">
-        <v>0.703041014361947</v>
+        <v>0.695598573402054</v>
       </c>
       <c r="U10" t="n">
-        <v>0.280611488809424</v>
+        <v>0.293013260655392</v>
       </c>
       <c r="V10" t="n">
-        <v>0.226152482983681</v>
+        <v>0.368740148857804</v>
       </c>
       <c r="W10" t="n">
-        <v>0.405809793872041</v>
+        <v>0.144057612298694</v>
       </c>
       <c r="X10" t="n">
-        <v>0.0941118852351122</v>
+        <v>0.0932292597638777</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.349037917058714</v>
+        <v>0.374244747658632</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.52239978010311</v>
+        <v>0.23653211670786</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.237294328597067</v>
+        <v>0.531090793021797</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.571863326111119</v>
+        <v>0.558366936228345</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.407541134295432</v>
+        <v>0.417486901369611</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.260185678830775</v>
+        <v>0.267820571743726</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.185233936942734</v>
+        <v>0.158501700523945</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.14703924993106</v>
+        <v>0.156190826362717</v>
       </c>
       <c r="AG10" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="AH10" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="AI10" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AJ10" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" t="s">
         <v>91</v>
-      </c>
-      <c r="B11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C11" t="s">
-        <v>93</v>
-      </c>
-      <c r="D11" t="s">
-        <v>87</v>
       </c>
       <c r="E11" t="n">
         <v>40.361706</v>
@@ -1962,78 +1974,78 @@
         <v>0.134753357098093</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.289248161493874</v>
+        <v>0.322589097913378</v>
       </c>
       <c r="R11" t="n">
-        <v>0.345406163537031</v>
+        <v>0.276491459888598</v>
       </c>
       <c r="S11" t="n">
-        <v>0.230531973387848</v>
+        <v>0.191812959034086</v>
       </c>
       <c r="T11" t="n">
-        <v>0.762114125868153</v>
+        <v>0.733923913517394</v>
       </c>
       <c r="U11" t="n">
-        <v>0.524212924672261</v>
+        <v>0.437540070673498</v>
       </c>
       <c r="V11" t="n">
-        <v>0.351366380888303</v>
+        <v>0.461823300441626</v>
       </c>
       <c r="W11" t="n">
-        <v>0.370274083266828</v>
+        <v>0.245099686407627</v>
       </c>
       <c r="X11" t="n">
-        <v>0.153175016973061</v>
+        <v>0.17182457727252</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.244790018145876</v>
+        <v>0.194328219349607</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.216391224379916</v>
+        <v>0.384845734290665</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.455742507614012</v>
+        <v>0.457802224444644</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.378950540526822</v>
+        <v>0.344782795954168</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.359838220424671</v>
+        <v>0.483310966081441</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.322555381928486</v>
+        <v>0.355275301038698</v>
       </c>
       <c r="AE11" t="n">
-        <v>0.283515028954867</v>
+        <v>0.12132365107087</v>
       </c>
       <c r="AF11" t="n">
-        <v>0.0340913686919754</v>
+        <v>0.0400900818089898</v>
       </c>
       <c r="AG11" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="AH11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AI11" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="AJ11" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B12" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C12" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D12" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E12" t="n">
         <v>40.353131</v>
@@ -2120,30 +2132,30 @@
         <v>0.0356117290192113</v>
       </c>
       <c r="AG12" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="AH12" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AI12" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="AJ12" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D13" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E13" t="n">
         <v>40.38491</v>
@@ -2182,10 +2194,10 @@
         <v>0.169647235699781</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.325393569159018</v>
+        <v>0.325398497441816</v>
       </c>
       <c r="R13" t="n">
-        <v>0.202048929206734</v>
+        <v>0.20205477760645</v>
       </c>
       <c r="S13" t="n">
         <v>0.558025693418098</v>
@@ -2194,10 +2206,10 @@
         <v>0.590848472137417</v>
       </c>
       <c r="U13" t="n">
-        <v>0.385276069448176</v>
+        <v>0.385276907988128</v>
       </c>
       <c r="V13" t="n">
-        <v>0.229039577238636</v>
+        <v>0.229054396800763</v>
       </c>
       <c r="W13" t="n">
         <v>0.534493742518764</v>
@@ -2206,10 +2218,10 @@
         <v>0.126235064768519</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.311205972216737</v>
+        <v>0.311192618051835</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.55639168863251</v>
+        <v>0.556384942524911</v>
       </c>
       <c r="AA13" t="n">
         <v>0.120862340052599</v>
@@ -2218,10 +2230,10 @@
         <v>0.419156170374463</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.493390936666973</v>
+        <v>0.493354168581671</v>
       </c>
       <c r="AD13" t="n">
-        <v>0.359678279253608</v>
+        <v>0.35971504733891</v>
       </c>
       <c r="AE13" t="n">
         <v>0.0850795109844655</v>
@@ -2230,30 +2242,30 @@
         <v>0.0618512730949536</v>
       </c>
       <c r="AG13" t="s">
-        <v>104</v>
+        <v>47</v>
       </c>
       <c r="AH13" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="AI13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AJ13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B14" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E14" t="n">
         <v>40.328281</v>
@@ -2292,61 +2304,61 @@
         <v>0.137882238499753</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.29882428487279</v>
+        <v>0.298817717114556</v>
       </c>
       <c r="R14" t="n">
-        <v>0.157559664937524</v>
+        <v>0.157550459912774</v>
       </c>
       <c r="S14" t="n">
-        <v>0.430997275471134</v>
+        <v>0.430999992027378</v>
       </c>
       <c r="T14" t="n">
-        <v>0.63872132224914</v>
+        <v>0.638738401262217</v>
       </c>
       <c r="U14" t="n">
-        <v>0.35122693863842</v>
+        <v>0.35122222148803</v>
       </c>
       <c r="V14" t="n">
-        <v>0.217829860403129</v>
+        <v>0.217815127306559</v>
       </c>
       <c r="W14" t="n">
-        <v>0.478118420244124</v>
+        <v>0.478114706106039</v>
       </c>
       <c r="X14" t="n">
-        <v>0.0827147002890197</v>
+        <v>0.082703336366558</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.346179528457546</v>
+        <v>0.346190493697637</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.495623768608962</v>
+        <v>0.495629936240767</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.18889976021098</v>
+        <v>0.188900415235752</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.474337272987963</v>
+        <v>0.474356054250311</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.405871863222723</v>
+        <v>0.405915984925085</v>
       </c>
       <c r="AD14" t="n">
-        <v>0.295131905506021</v>
+        <v>0.295091460612189</v>
       </c>
       <c r="AE14" t="n">
-        <v>0.23840610350216</v>
+        <v>0.23840978031069</v>
       </c>
       <c r="AF14" t="n">
-        <v>0.0605901277690964</v>
+        <v>0.060582774152036</v>
       </c>
       <c r="AG14" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AH14" t="s">
         <v>42</v>
       </c>
       <c r="AI14" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="AJ14" t="s">
         <v>43</v>
@@ -2354,16 +2366,16 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C15" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D15" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E15" t="n">
         <v>40.321026</v>
@@ -2402,49 +2414,49 @@
         <v>0.135458622877551</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.292080375933529</v>
+        <v>0.292092629808491</v>
       </c>
       <c r="R15" t="n">
-        <v>0.428311830437071</v>
+        <v>0.428311847479398</v>
       </c>
       <c r="S15" t="n">
-        <v>0.15592231129015</v>
+        <v>0.155937391541153</v>
       </c>
       <c r="T15" t="n">
         <v>0.661641591481738</v>
       </c>
       <c r="U15" t="n">
-        <v>0.347413671474267</v>
+        <v>0.34742573031661</v>
       </c>
       <c r="V15" t="n">
-        <v>0.456895489929101</v>
+        <v>0.456895667451419</v>
       </c>
       <c r="W15" t="n">
-        <v>0.189478191521914</v>
+        <v>0.189500164328434</v>
       </c>
       <c r="X15" t="n">
         <v>0.0812793185071385</v>
       </c>
       <c r="Y15" t="n">
-        <v>0.37227171221953</v>
+        <v>0.372266338700046</v>
       </c>
       <c r="Z15" t="n">
-        <v>0.20256998294444</v>
+        <v>0.20256911429179</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.510326129093632</v>
+        <v>0.510294841833704</v>
       </c>
       <c r="AB15" t="n">
         <v>0.481926044610384</v>
       </c>
       <c r="AC15" t="n">
-        <v>0.447087048441952</v>
+        <v>0.447030057909734</v>
       </c>
       <c r="AD15" t="n">
-        <v>0.30994576707418</v>
+        <v>0.309943928669914</v>
       </c>
       <c r="AE15" t="n">
-        <v>0.184112510341024</v>
+        <v>0.184171339277507</v>
       </c>
       <c r="AF15" t="n">
         <v>0.058854674142844</v>
@@ -2453,27 +2465,27 @@
         <v>41</v>
       </c>
       <c r="AH15" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="AI15" t="s">
         <v>42</v>
       </c>
       <c r="AJ15" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D16" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E16" t="n">
         <v>40.343974</v>
@@ -2560,30 +2572,30 @@
         <v>0.166750620461439</v>
       </c>
       <c r="AG16" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AH16" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="AI16" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AJ16" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E17" t="n">
         <v>40.342717</v>
@@ -2622,64 +2634,64 @@
         <v>0.144644469374759</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.339031832334921</v>
+        <v>0.339678597503287</v>
       </c>
       <c r="R17" t="n">
-        <v>0.52958372822167</v>
+        <v>0.530503122548382</v>
       </c>
       <c r="S17" t="n">
-        <v>0.702315576925458</v>
+        <v>0.702316626659081</v>
       </c>
       <c r="T17" t="n">
-        <v>0.177921169342105</v>
+        <v>0.178548136532459</v>
       </c>
       <c r="U17" t="n">
-        <v>0.262604386419732</v>
+        <v>0.263108358935227</v>
       </c>
       <c r="V17" t="n">
-        <v>0.346428783569233</v>
+        <v>0.346706682755228</v>
       </c>
       <c r="W17" t="n">
-        <v>0.0876092333192684</v>
+        <v>0.0876216733096653</v>
       </c>
       <c r="X17" t="n">
-        <v>0.131672441686606</v>
+        <v>0.132104272194292</v>
       </c>
       <c r="Y17" t="n">
-        <v>0.416845703855392</v>
+        <v>0.416056768856574</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.263114292064012</v>
+        <v>0.262624238844213</v>
       </c>
       <c r="AA17" t="n">
-        <v>0.547609883320447</v>
+        <v>0.547597315165699</v>
       </c>
       <c r="AB17" t="n">
-        <v>0.588084725952029</v>
+        <v>0.587436409106286</v>
       </c>
       <c r="AC17" t="n">
-        <v>0.380751907344425</v>
+        <v>0.381862303520544</v>
       </c>
       <c r="AD17" t="n">
-        <v>0.296661457854582</v>
+        <v>0.294379998161596</v>
       </c>
       <c r="AE17" t="n">
-        <v>0.164529828109201</v>
+        <v>0.164540858534792</v>
       </c>
       <c r="AF17" t="n">
-        <v>0.158056806691792</v>
+        <v>0.159216839783068</v>
       </c>
       <c r="AG17" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AH17" t="s">
-        <v>104</v>
+        <v>47</v>
       </c>
       <c r="AI17" t="s">
-        <v>123</v>
+        <v>74</v>
       </c>
       <c r="AJ17" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18">
@@ -2693,7 +2705,7 @@
         <v>126</v>
       </c>
       <c r="D18" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E18" t="n">
         <v>40.345588</v>
@@ -2732,78 +2744,78 @@
         <v>0.141867623839505</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.36275445808786</v>
+        <v>0.362478079632924</v>
       </c>
       <c r="R18" t="n">
-        <v>0.541023369448056</v>
+        <v>0.540671167025388</v>
       </c>
       <c r="S18" t="n">
-        <v>0.209632175764592</v>
+        <v>0.209389274923546</v>
       </c>
       <c r="T18" t="n">
-        <v>0.699444544294824</v>
+        <v>0.699451622021524</v>
       </c>
       <c r="U18" t="n">
-        <v>0.267450098007967</v>
+        <v>0.267268410293893</v>
       </c>
       <c r="V18" t="n">
-        <v>0.356711114587473</v>
+        <v>0.356502049499612</v>
       </c>
       <c r="W18" t="n">
-        <v>0.141966096914688</v>
+        <v>0.141766407373292</v>
       </c>
       <c r="X18" t="n">
-        <v>0.0898061488971261</v>
+        <v>0.0897832769336292</v>
       </c>
       <c r="Y18" t="n">
-        <v>0.387835839057397</v>
+        <v>0.388174118883234</v>
       </c>
       <c r="Z18" t="n">
-        <v>0.253297003327624</v>
+        <v>0.253510706914372</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.552991891505294</v>
+        <v>0.553167503638604</v>
       </c>
       <c r="AB18" t="n">
-        <v>0.547300703316466</v>
+        <v>0.547380370407727</v>
       </c>
       <c r="AC18" t="n">
-        <v>0.376069491681221</v>
+        <v>0.375584152955235</v>
       </c>
       <c r="AD18" t="n">
-        <v>0.26722309035757</v>
+        <v>0.268259950363085</v>
       </c>
       <c r="AE18" t="n">
-        <v>0.182954315654012</v>
+        <v>0.182459784906701</v>
       </c>
       <c r="AF18" t="n">
-        <v>0.173753102307197</v>
+        <v>0.173696111774979</v>
       </c>
       <c r="AG18" t="s">
-        <v>127</v>
+        <v>71</v>
       </c>
       <c r="AH18" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="AI18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AJ18" t="s">
-        <v>123</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B19" t="s">
         <v>128</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>129</v>
       </c>
-      <c r="C19" t="s">
-        <v>130</v>
-      </c>
       <c r="D19" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E19" t="n">
         <v>40.334348</v>
@@ -2890,16 +2902,126 @@
         <v>0.138685540950455</v>
       </c>
       <c r="AG19" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AH19" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI19" t="s">
         <v>131</v>
       </c>
-      <c r="AI19" t="s">
+      <c r="AJ19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
         <v>132</v>
       </c>
-      <c r="AJ19" t="s">
-        <v>123</v>
+      <c r="B20" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" t="s">
+        <v>135</v>
+      </c>
+      <c r="E20" t="n">
+        <v>40.35151</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-74.660325</v>
+      </c>
+      <c r="G20" t="n">
+        <v>40.357259</v>
+      </c>
+      <c r="H20" t="n">
+        <v>-74.671573</v>
+      </c>
+      <c r="I20" t="n">
+        <v>40.34662</v>
+      </c>
+      <c r="J20" t="n">
+        <v>-74.648996</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.17792330943395</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.128004148233067</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.388235294117647</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.142405744188794</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0.35922062047724</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0.530102122973561</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0.698993810031887</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0.232969249181813</v>
+      </c>
+      <c r="U20" t="n">
+        <v>0.277770693838942</v>
+      </c>
+      <c r="V20" t="n">
+        <v>0.352560683359115</v>
+      </c>
+      <c r="W20" t="n">
+        <v>0.0899407118788011</v>
+      </c>
+      <c r="X20" t="n">
+        <v>0.140067819203644</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>0.386128782448231</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>0.251671071604821</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>0.558917184018112</v>
+      </c>
+      <c r="AB20" t="n">
+        <v>0.535071880989868</v>
+      </c>
+      <c r="AC20" t="n">
+        <v>0.375641143487453</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>0.271809908998989</v>
+      </c>
+      <c r="AE20" t="n">
+        <v>0.177744277966725</v>
+      </c>
+      <c r="AF20" t="n">
+        <v>0.174804669546833</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>136</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2918,10 +3040,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
@@ -2929,7 +3051,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3">
@@ -2937,7 +3059,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4">
@@ -2945,7 +3067,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5">
@@ -2953,7 +3075,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6">
@@ -2961,7 +3083,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7">
@@ -2969,7 +3091,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8">
@@ -2977,7 +3099,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9">
@@ -2985,7 +3107,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10">
@@ -2993,7 +3115,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11">
@@ -3001,7 +3123,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12">
@@ -3009,7 +3131,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13">
@@ -3017,7 +3139,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14">
@@ -3025,7 +3147,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15">
@@ -3033,7 +3155,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16">
@@ -3041,7 +3163,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17">
@@ -3049,7 +3171,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18">
@@ -3057,7 +3179,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19">
@@ -3065,7 +3187,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20">
@@ -3073,7 +3195,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21">
@@ -3081,7 +3203,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22">
@@ -3089,7 +3211,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23">
@@ -3097,7 +3219,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24">
@@ -3105,7 +3227,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25">
@@ -3113,7 +3235,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26">
@@ -3121,7 +3243,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27">
@@ -3129,7 +3251,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28">
@@ -3137,7 +3259,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29">
@@ -3145,7 +3267,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30">
@@ -3153,7 +3275,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31">
@@ -3161,7 +3283,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32">
@@ -3169,7 +3291,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33">
@@ -3177,7 +3299,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34">
@@ -3185,7 +3307,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35">
@@ -3193,7 +3315,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36">
@@ -3201,7 +3323,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37">
@@ -3209,7 +3331,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>